<commit_message>
Update for new LDF(0x34 & 0x35)
</commit_message>
<xml_diff>
--- a/020_System/40_Design/GoodProjectAngel.xlsx
+++ b/020_System/40_Design/GoodProjectAngel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\00_Workspace\00_YTP_GoodProject\020_System\40_Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\050_Workspace\010_YTP_SENT\020_System\40_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F340AD7-E09F-4676-9A08-20C138AAD915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA7A661-0676-4521-AF89-6BC9CCBFC0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="90">
   <si>
     <t>Step1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -354,23 +354,31 @@
   </si>
   <si>
     <t>1.0</t>
+  </si>
+  <si>
+    <t>First</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Second</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -399,8 +407,26 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -410,6 +436,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,7 +521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="1" borderId="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -475,6 +543,29 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -757,302 +848,638 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E6:K23"/>
+  <dimension ref="A6:O33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.75" customWidth="1"/>
+    <col min="15" max="15" width="77.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="5:11">
-      <c r="F6" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>0</v>
       </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
       <c r="G6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="5:11">
-      <c r="E7" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="F7">
+      <c r="B7">
         <v>100</v>
       </c>
-      <c r="G7">
+      <c r="C7">
         <v>20</v>
       </c>
-      <c r="H7">
-        <f>ROUND(40950*F7/340,0)</f>
+      <c r="D7">
+        <f>ROUND(40950*B7/340,0)</f>
         <v>12044</v>
       </c>
-      <c r="I7">
-        <f>ROUND(40950*G7/340,0)</f>
+      <c r="E7">
+        <f>ROUND(40950*C7/340,0)</f>
         <v>2409</v>
       </c>
-      <c r="K7" t="str">
-        <f>"  {" &amp; H7 &amp; ", " &amp; I7 &amp;"},  /* First step is " &amp; F7 &amp; " Second step is " &amp;G7 &amp; " */"</f>
+      <c r="G7" t="str">
+        <f>"  {" &amp; D7 &amp; ", " &amp; E7 &amp;"},  /* First step is " &amp; B7 &amp; " Second step is " &amp;C7 &amp; " */"</f>
         <v xml:space="preserve">  {12044, 2409},  /* First step is 100 Second step is 20 */</v>
       </c>
-    </row>
-    <row r="8" spans="5:11">
-      <c r="E8" t="s">
+      <c r="N7">
+        <v>340</v>
+      </c>
+      <c r="O7">
+        <v>40950</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="F8">
+      <c r="B8">
         <v>300</v>
       </c>
-      <c r="G8">
+      <c r="C8">
         <v>30</v>
       </c>
-      <c r="H8">
-        <f t="shared" ref="H8:H14" si="0">ROUND(40950*F8/340,0)</f>
+      <c r="D8">
+        <f t="shared" ref="D8:D14" si="0">ROUND(40950*B8/340,0)</f>
         <v>36132</v>
       </c>
-      <c r="I8">
-        <f t="shared" ref="I8:I14" si="1">ROUND(40950*G8/340,0)</f>
+      <c r="E8">
+        <f t="shared" ref="E8:E14" si="1">ROUND(40950*C8/340,0)</f>
         <v>3613</v>
       </c>
-      <c r="K8" t="str">
-        <f t="shared" ref="K8:K14" si="2">"  {" &amp; H8 &amp; ", " &amp; I8 &amp;"},  /* First step is " &amp; F8 &amp; " Second step is " &amp;G8 &amp; " */"</f>
+      <c r="G8" t="str">
+        <f t="shared" ref="G8:G14" si="2">"  {" &amp; D8 &amp; ", " &amp; E8 &amp;"},  /* First step is " &amp; B8 &amp; " Second step is " &amp;C8 &amp; " */"</f>
         <v xml:space="preserve">  {36132, 3613},  /* First step is 300 Second step is 30 */</v>
       </c>
-    </row>
-    <row r="9" spans="5:11">
-      <c r="E9" t="s">
+      <c r="N8">
+        <v>360</v>
+      </c>
+      <c r="O8">
+        <f>N8*O7/N7</f>
+        <v>43358.823529411762</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="F9">
+      <c r="B9">
         <v>200</v>
       </c>
-      <c r="G9">
+      <c r="C9">
         <v>50</v>
       </c>
-      <c r="H9">
+      <c r="D9">
         <f t="shared" si="0"/>
         <v>24088</v>
       </c>
-      <c r="I9">
+      <c r="E9">
         <f t="shared" si="1"/>
         <v>6022</v>
       </c>
-      <c r="K9" t="str">
+      <c r="G9" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">  {24088, 6022},  /* First step is 200 Second step is 50 */</v>
       </c>
     </row>
-    <row r="10" spans="5:11">
-      <c r="E10" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="F10">
+      <c r="B10">
         <v>110</v>
       </c>
-      <c r="G10">
+      <c r="C10">
         <v>80</v>
       </c>
-      <c r="H10">
+      <c r="D10">
         <f t="shared" si="0"/>
         <v>13249</v>
       </c>
-      <c r="I10">
+      <c r="E10">
         <f t="shared" si="1"/>
         <v>9635</v>
       </c>
-      <c r="K10" t="str">
+      <c r="G10" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">  {13249, 9635},  /* First step is 110 Second step is 80 */</v>
       </c>
     </row>
-    <row r="11" spans="5:11">
-      <c r="E11" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="F11">
+      <c r="B11">
         <v>320</v>
       </c>
-      <c r="G11">
+      <c r="C11">
         <v>250</v>
       </c>
-      <c r="H11">
+      <c r="D11">
         <f t="shared" si="0"/>
         <v>38541</v>
       </c>
-      <c r="I11">
+      <c r="E11">
         <f t="shared" si="1"/>
         <v>30110</v>
       </c>
-      <c r="K11" t="str">
+      <c r="G11" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">  {38541, 30110},  /* First step is 320 Second step is 250 */</v>
       </c>
     </row>
-    <row r="12" spans="5:11">
-      <c r="E12" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="F12">
+      <c r="B12">
         <v>320</v>
       </c>
-      <c r="G12">
+      <c r="C12">
         <v>50</v>
       </c>
-      <c r="H12">
+      <c r="D12">
         <f t="shared" si="0"/>
         <v>38541</v>
       </c>
-      <c r="I12">
+      <c r="E12">
         <f t="shared" si="1"/>
         <v>6022</v>
       </c>
-      <c r="K12" t="str">
+      <c r="G12" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">  {38541, 6022},  /* First step is 320 Second step is 50 */</v>
       </c>
     </row>
-    <row r="13" spans="5:11">
-      <c r="E13" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="F13">
+      <c r="B13">
         <v>270</v>
       </c>
-      <c r="G13">
+      <c r="C13">
         <v>180</v>
       </c>
-      <c r="H13">
+      <c r="D13">
         <f t="shared" si="0"/>
         <v>32519</v>
       </c>
-      <c r="I13">
+      <c r="E13">
         <f t="shared" si="1"/>
         <v>21679</v>
       </c>
-      <c r="K13" t="str">
+      <c r="G13" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">  {32519, 21679},  /* First step is 270 Second step is 180 */</v>
       </c>
     </row>
-    <row r="14" spans="5:11">
-      <c r="E14" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="F14">
+      <c r="B14">
         <v>200</v>
       </c>
-      <c r="G14">
+      <c r="C14">
         <v>80</v>
       </c>
-      <c r="H14">
+      <c r="D14">
         <f t="shared" si="0"/>
         <v>24088</v>
       </c>
-      <c r="I14">
+      <c r="E14">
         <f t="shared" si="1"/>
         <v>9635</v>
       </c>
-      <c r="K14" t="str">
+      <c r="G14" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">  {24088, 9635},  /* First step is 200 Second step is 80 */</v>
       </c>
     </row>
-    <row r="16" spans="5:11">
-      <c r="G16">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C16">
         <v>100</v>
       </c>
-      <c r="H16">
-        <f>ROUND(40950*G16/340,0)</f>
+      <c r="D16">
+        <f>ROUND(40950*C16/340,0)</f>
         <v>12044</v>
       </c>
-      <c r="I16">
-        <f>ROUND(H16/10,0)</f>
+      <c r="E16">
+        <f>ROUND(D16/10,0)</f>
         <v>1204</v>
       </c>
-      <c r="J16" t="str">
-        <f>DEC2HEX(ROUND(H16/10,0))</f>
+      <c r="F16" t="str">
+        <f>DEC2HEX(ROUND(D16/10,0))</f>
         <v>4B4</v>
       </c>
     </row>
-    <row r="17" spans="7:10">
-      <c r="G17">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C17">
         <v>180</v>
       </c>
-      <c r="H17">
-        <f t="shared" ref="H17:H19" si="3">ROUND(40950*G17/340,0)</f>
+      <c r="D17">
+        <f t="shared" ref="D17:D18" si="3">ROUND(40950*C17/340,0)</f>
         <v>21679</v>
       </c>
-      <c r="I17">
-        <f t="shared" ref="I17:I19" si="4">ROUND(H17/10,0)</f>
+      <c r="E17">
+        <f t="shared" ref="E17:E18" si="4">ROUND(D17/10,0)</f>
         <v>2168</v>
       </c>
-      <c r="J17" t="str">
-        <f t="shared" ref="J17:J18" si="5">DEC2HEX(ROUND(H17/10,0))</f>
+      <c r="F17" t="str">
+        <f t="shared" ref="F17:F18" si="5">DEC2HEX(ROUND(D17/10,0))</f>
         <v>878</v>
       </c>
     </row>
-    <row r="18" spans="7:10">
-      <c r="G18">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C18">
         <v>460</v>
       </c>
-      <c r="H18">
+      <c r="D18">
         <f t="shared" si="3"/>
         <v>55403</v>
       </c>
-      <c r="I18">
+      <c r="E18">
         <f t="shared" si="4"/>
         <v>5540</v>
       </c>
-      <c r="J18" t="str">
+      <c r="F18" t="str">
         <f t="shared" si="5"/>
         <v>15A4</v>
       </c>
     </row>
-    <row r="19" spans="7:10">
-      <c r="G19">
-        <f>G18+360</f>
-        <v>820</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="3"/>
-        <v>98762</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="4"/>
-        <v>9876</v>
-      </c>
-      <c r="J19" t="str">
-        <f t="shared" ref="J19" si="6">DEC2HEX(ROUND(H19/10,0))</f>
-        <v>2694</v>
-      </c>
-    </row>
-    <row r="22" spans="7:10">
-      <c r="I22">
-        <v>340</v>
-      </c>
-      <c r="J22">
-        <v>40950</v>
-      </c>
-    </row>
-    <row r="23" spans="7:10">
-      <c r="I23">
-        <v>360</v>
-      </c>
-      <c r="J23">
-        <f>I23*J22/I22</f>
-        <v>43358.823529411762</v>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C25" s="11"/>
+      <c r="D25" s="12">
+        <v>0</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1</v>
+      </c>
+      <c r="F25" s="12">
+        <v>2</v>
+      </c>
+      <c r="G25" s="12">
+        <v>3</v>
+      </c>
+      <c r="H25" s="12">
+        <v>4</v>
+      </c>
+      <c r="I25" s="12">
+        <v>5</v>
+      </c>
+      <c r="J25" s="12">
+        <v>6</v>
+      </c>
+      <c r="K25" s="12">
+        <v>7</v>
+      </c>
+      <c r="L25" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="C26" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="13">
+        <v>200</v>
+      </c>
+      <c r="E26" s="13">
+        <v>230</v>
+      </c>
+      <c r="F26" s="13">
+        <v>200</v>
+      </c>
+      <c r="G26" s="13">
+        <v>80</v>
+      </c>
+      <c r="H26" s="13">
+        <v>230</v>
+      </c>
+      <c r="I26" s="13">
+        <v>250</v>
+      </c>
+      <c r="J26" s="13">
+        <v>200</v>
+      </c>
+      <c r="K26" s="13">
+        <v>150.5</v>
+      </c>
+      <c r="L26" s="13">
+        <v>180.8</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="C27" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="13">
+        <v>100</v>
+      </c>
+      <c r="E27" s="13">
+        <v>130</v>
+      </c>
+      <c r="F27" s="13">
+        <v>100</v>
+      </c>
+      <c r="G27" s="13">
+        <v>80</v>
+      </c>
+      <c r="H27" s="13">
+        <v>100</v>
+      </c>
+      <c r="I27" s="13">
+        <v>200</v>
+      </c>
+      <c r="J27" s="13">
+        <v>100</v>
+      </c>
+      <c r="K27" s="13">
+        <v>100</v>
+      </c>
+      <c r="L27" s="13">
+        <v>80.8</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C28" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="14">
+        <f>ROUND(40950*D26/340,0)</f>
+        <v>24088</v>
+      </c>
+      <c r="E28" s="14">
+        <f t="shared" ref="E28:K29" si="6">ROUND(40950*E26/340,0)</f>
+        <v>27701</v>
+      </c>
+      <c r="F28" s="14">
+        <f t="shared" si="6"/>
+        <v>24088</v>
+      </c>
+      <c r="G28" s="14">
+        <f t="shared" si="6"/>
+        <v>9635</v>
+      </c>
+      <c r="H28" s="14">
+        <f t="shared" si="6"/>
+        <v>27701</v>
+      </c>
+      <c r="I28" s="14">
+        <f t="shared" si="6"/>
+        <v>30110</v>
+      </c>
+      <c r="J28" s="14">
+        <f t="shared" si="6"/>
+        <v>24088</v>
+      </c>
+      <c r="K28" s="14">
+        <f t="shared" si="6"/>
+        <v>18126</v>
+      </c>
+      <c r="L28" s="14">
+        <f t="shared" ref="L28" si="7">ROUND(40950*L26/340,0)</f>
+        <v>21776</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C29" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="14">
+        <f>ROUND(40950*D27/340,0)</f>
+        <v>12044</v>
+      </c>
+      <c r="E29" s="14">
+        <f t="shared" si="6"/>
+        <v>15657</v>
+      </c>
+      <c r="F29" s="14">
+        <f t="shared" si="6"/>
+        <v>12044</v>
+      </c>
+      <c r="G29" s="14">
+        <f t="shared" si="6"/>
+        <v>9635</v>
+      </c>
+      <c r="H29" s="14">
+        <f t="shared" si="6"/>
+        <v>12044</v>
+      </c>
+      <c r="I29" s="14">
+        <f t="shared" si="6"/>
+        <v>24088</v>
+      </c>
+      <c r="J29" s="14">
+        <f t="shared" si="6"/>
+        <v>12044</v>
+      </c>
+      <c r="K29" s="14">
+        <f t="shared" si="6"/>
+        <v>12044</v>
+      </c>
+      <c r="L29" s="14">
+        <f t="shared" ref="L29" si="8">ROUND(40950*L27/340,0)</f>
+        <v>9732</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="C30" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="15">
+        <f>ROUND(D28/10,0)</f>
+        <v>2409</v>
+      </c>
+      <c r="E30" s="15">
+        <f t="shared" ref="E30:K31" si="9">ROUND(E28/10,0)</f>
+        <v>2770</v>
+      </c>
+      <c r="F30" s="15">
+        <f t="shared" si="9"/>
+        <v>2409</v>
+      </c>
+      <c r="G30" s="15">
+        <f t="shared" si="9"/>
+        <v>964</v>
+      </c>
+      <c r="H30" s="15">
+        <f t="shared" si="9"/>
+        <v>2770</v>
+      </c>
+      <c r="I30" s="15">
+        <f t="shared" si="9"/>
+        <v>3011</v>
+      </c>
+      <c r="J30" s="15">
+        <f t="shared" si="9"/>
+        <v>2409</v>
+      </c>
+      <c r="K30" s="15">
+        <f t="shared" si="9"/>
+        <v>1813</v>
+      </c>
+      <c r="L30" s="15">
+        <f t="shared" ref="L30" si="10">ROUND(L28/10,0)</f>
+        <v>2178</v>
+      </c>
+      <c r="N30" t="str">
+        <f>D30&amp;", "&amp;E30&amp;", "&amp;F30&amp;", "&amp;G30&amp;", "&amp;H30&amp;", "&amp;I30&amp;", "&amp;J30&amp;", "&amp;K30&amp;", "&amp;L30</f>
+        <v>2409, 2770, 2409, 964, 2770, 3011, 2409, 1813, 2178</v>
+      </c>
+      <c r="O30" s="10" t="str">
+        <f>"word calibration"&amp;C30&amp;"PosArray[9] = {"&amp;N30&amp;"};"</f>
+        <v>word calibrationFirstPosArray[9] = {2409, 2770, 2409, 964, 2770, 3011, 2409, 1813, 2178};</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="C31" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="16">
+        <f>ROUND(D29/10,0)</f>
+        <v>1204</v>
+      </c>
+      <c r="E31" s="16">
+        <f t="shared" si="9"/>
+        <v>1566</v>
+      </c>
+      <c r="F31" s="16">
+        <f t="shared" si="9"/>
+        <v>1204</v>
+      </c>
+      <c r="G31" s="16">
+        <f t="shared" si="9"/>
+        <v>964</v>
+      </c>
+      <c r="H31" s="16">
+        <f t="shared" si="9"/>
+        <v>1204</v>
+      </c>
+      <c r="I31" s="16">
+        <f t="shared" si="9"/>
+        <v>2409</v>
+      </c>
+      <c r="J31" s="16">
+        <f t="shared" si="9"/>
+        <v>1204</v>
+      </c>
+      <c r="K31" s="16">
+        <f t="shared" si="9"/>
+        <v>1204</v>
+      </c>
+      <c r="L31" s="16">
+        <f t="shared" ref="L31" si="11">ROUND(L29/10,0)</f>
+        <v>973</v>
+      </c>
+      <c r="N31" t="str">
+        <f>D31&amp;", "&amp;E31&amp;", "&amp;F31&amp;", "&amp;G31&amp;", "&amp;H31&amp;", "&amp;I31&amp;", "&amp;J31&amp;", "&amp;K31&amp;", "&amp;L31</f>
+        <v>1204, 1566, 1204, 964, 1204, 2409, 1204, 1204, 973</v>
+      </c>
+      <c r="O31" s="10" t="str">
+        <f>"word calibration"&amp;C31&amp;"PosArray[9] = {"&amp;N31&amp;"};"</f>
+        <v>word calibrationSecondPosArray[9] = {1204, 1566, 1204, 964, 1204, 2409, 1204, 1204, 973};</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C32" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" s="17" t="str">
+        <f>DEC2HEX(ROUND(D28/10,0))</f>
+        <v>969</v>
+      </c>
+      <c r="E32" s="17" t="str">
+        <f t="shared" ref="E32:K32" si="12">DEC2HEX(ROUND(E28/10,0))</f>
+        <v>AD2</v>
+      </c>
+      <c r="F32" s="17" t="str">
+        <f t="shared" si="12"/>
+        <v>969</v>
+      </c>
+      <c r="G32" s="17" t="str">
+        <f t="shared" si="12"/>
+        <v>3C4</v>
+      </c>
+      <c r="H32" s="17" t="str">
+        <f t="shared" si="12"/>
+        <v>AD2</v>
+      </c>
+      <c r="I32" s="17" t="str">
+        <f t="shared" si="12"/>
+        <v>BC3</v>
+      </c>
+      <c r="J32" s="17" t="str">
+        <f t="shared" si="12"/>
+        <v>969</v>
+      </c>
+      <c r="K32" s="17" t="str">
+        <f t="shared" si="12"/>
+        <v>715</v>
+      </c>
+      <c r="L32" s="17" t="str">
+        <f t="shared" ref="L32" si="13">DEC2HEX(ROUND(L28/10,0))</f>
+        <v>882</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C33" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="18" t="str">
+        <f>DEC2HEX(ROUND(D29/10,0))</f>
+        <v>4B4</v>
+      </c>
+      <c r="E33" s="18" t="str">
+        <f t="shared" ref="E33:K33" si="14">DEC2HEX(ROUND(E29/10,0))</f>
+        <v>61E</v>
+      </c>
+      <c r="F33" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>4B4</v>
+      </c>
+      <c r="G33" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>3C4</v>
+      </c>
+      <c r="H33" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>4B4</v>
+      </c>
+      <c r="I33" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>969</v>
+      </c>
+      <c r="J33" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>4B4</v>
+      </c>
+      <c r="K33" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>4B4</v>
+      </c>
+      <c r="L33" s="18" t="str">
+        <f t="shared" ref="L33" si="15">DEC2HEX(ROUND(L29/10,0))</f>
+        <v>3CD</v>
       </c>
     </row>
   </sheetData>
@@ -1066,34 +1493,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFDF32A-9B3A-4F81-AD96-0784476499BF}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="9" style="3"/>
-    <col min="3" max="3" width="49.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.25" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.36328125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="26.90625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.7265625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="17.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.08984375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.6328125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="11.36328125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="17.7265625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="16.7265625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="82.08984375" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="8.7265625" style="3"/>
+    <col min="6" max="6" width="7.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="26.875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.75" style="3" customWidth="1"/>
+    <col min="11" max="11" width="17.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="11.375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="17.75" style="3" customWidth="1"/>
+    <col min="17" max="17" width="16.75" style="3" customWidth="1"/>
+    <col min="18" max="18" width="82.125" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="8.75" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
@@ -1149,7 +1576,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
@@ -1203,7 +1630,7 @@
       </c>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="28">
+    <row r="4" spans="1:18" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1247,7 +1674,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1289,7 +1716,7 @@
       </c>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1331,7 +1758,7 @@
       </c>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1373,7 +1800,7 @@
       </c>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1393,7 +1820,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1413,7 +1840,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
         <v>40</v>
@@ -1465,7 +1892,7 @@
       </c>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1507,7 +1934,7 @@
       </c>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1549,7 +1976,7 @@
       </c>
       <c r="R12" s="7"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1569,7 +1996,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="7"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="6" t="s">
         <v>83</v>
@@ -1621,7 +2048,7 @@
       </c>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18" ht="28">
+    <row r="15" spans="1:18" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1665,7 +2092,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1685,7 +2112,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="7"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1705,7 +2132,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="7"/>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -1753,7 +2180,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1789,7 +2216,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1809,7 +2236,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="7"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="6" t="s">
         <v>51</v>
@@ -1855,7 +2282,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1891,7 +2318,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1912,6 +2339,7 @@
       <c r="R23" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Release SW_1.1 1.Add LIN InitRequest signal 2.Add LIN TargetPosEnable signal 3.Fix issue that Sent position not stable 4.Change SW version number to 1.1
</commit_message>
<xml_diff>
--- a/020_System/40_Design/GoodProjectAngel.xlsx
+++ b/020_System/40_Design/GoodProjectAngel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\050_Workspace\010_YTP_SENT\020_System\40_Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\00_Workspace\00_YTP_GoodProject\020_System\40_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA7A661-0676-4521-AF89-6BC9CCBFC0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE6EA53-DC6E-4822-92A6-9BD1D4E5D9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,17 +368,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -411,7 +411,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -420,7 +420,7 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -848,20 +848,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A6:O33"/>
+  <dimension ref="A6:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.75" customWidth="1"/>
-    <col min="15" max="15" width="77.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7265625" customWidth="1"/>
+    <col min="15" max="15" width="77.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -878,7 +878,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -907,7 +907,7 @@
         <v>40950</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -937,7 +937,7 @@
         <v>43358.823529411762</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -960,7 +960,7 @@
         <v xml:space="preserve">  {24088, 6022},  /* First step is 200 Second step is 50 */</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -983,7 +983,7 @@
         <v xml:space="preserve">  {13249, 9635},  /* First step is 110 Second step is 80 */</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v xml:space="preserve">  {38541, 30110},  /* First step is 320 Second step is 250 */</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v xml:space="preserve">  {38541, 6022},  /* First step is 320 Second step is 50 */</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v xml:space="preserve">  {32519, 21679},  /* First step is 270 Second step is 180 */</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v xml:space="preserve">  {24088, 9635},  /* First step is 200 Second step is 80 */</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15">
       <c r="C16">
         <v>100</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>4B4</v>
       </c>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:15">
       <c r="C17">
         <v>180</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:15">
       <c r="C18">
         <v>460</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>15A4</v>
       </c>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:15">
       <c r="C25" s="11"/>
       <c r="D25" s="12">
         <v>0</v>
@@ -1156,7 +1156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="3:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:15" ht="18.5">
       <c r="C26" s="11" t="s">
         <v>88</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>180.8</v>
       </c>
     </row>
-    <row r="27" spans="3:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:15" ht="18.5">
       <c r="C27" s="11" t="s">
         <v>89</v>
       </c>
@@ -1199,28 +1199,28 @@
         <v>130</v>
       </c>
       <c r="F27" s="13">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G27" s="13">
         <v>80</v>
       </c>
       <c r="H27" s="13">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I27" s="13">
         <v>200</v>
       </c>
       <c r="J27" s="13">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K27" s="13">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="L27" s="13">
         <v>80.8</v>
       </c>
     </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:15">
       <c r="C28" s="11" t="s">
         <v>88</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>21776</v>
       </c>
     </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:15">
       <c r="C29" s="11" t="s">
         <v>89</v>
       </c>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="F29" s="14">
         <f t="shared" si="6"/>
-        <v>12044</v>
+        <v>18066</v>
       </c>
       <c r="G29" s="14">
         <f t="shared" si="6"/>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="H29" s="14">
         <f t="shared" si="6"/>
-        <v>12044</v>
+        <v>9635</v>
       </c>
       <c r="I29" s="14">
         <f t="shared" si="6"/>
@@ -1291,18 +1291,18 @@
       </c>
       <c r="J29" s="14">
         <f t="shared" si="6"/>
-        <v>12044</v>
+        <v>6022</v>
       </c>
       <c r="K29" s="14">
         <f t="shared" si="6"/>
-        <v>12044</v>
+        <v>8431</v>
       </c>
       <c r="L29" s="14">
         <f t="shared" ref="L29" si="8">ROUND(40950*L27/340,0)</f>
         <v>9732</v>
       </c>
     </row>
-    <row r="30" spans="3:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:15" ht="18.5">
       <c r="C30" s="11" t="s">
         <v>88</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>word calibrationFirstPosArray[9] = {2409, 2770, 2409, 964, 2770, 3011, 2409, 1813, 2178};</v>
       </c>
     </row>
-    <row r="31" spans="3:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:15" ht="18.5">
       <c r="C31" s="11" t="s">
         <v>89</v>
       </c>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="F31" s="16">
         <f t="shared" si="9"/>
-        <v>1204</v>
+        <v>1807</v>
       </c>
       <c r="G31" s="16">
         <f t="shared" si="9"/>
@@ -1373,7 +1373,7 @@
       </c>
       <c r="H31" s="16">
         <f t="shared" si="9"/>
-        <v>1204</v>
+        <v>964</v>
       </c>
       <c r="I31" s="16">
         <f t="shared" si="9"/>
@@ -1381,11 +1381,11 @@
       </c>
       <c r="J31" s="16">
         <f t="shared" si="9"/>
-        <v>1204</v>
+        <v>602</v>
       </c>
       <c r="K31" s="16">
         <f t="shared" si="9"/>
-        <v>1204</v>
+        <v>843</v>
       </c>
       <c r="L31" s="16">
         <f t="shared" ref="L31" si="11">ROUND(L29/10,0)</f>
@@ -1393,14 +1393,14 @@
       </c>
       <c r="N31" t="str">
         <f>D31&amp;", "&amp;E31&amp;", "&amp;F31&amp;", "&amp;G31&amp;", "&amp;H31&amp;", "&amp;I31&amp;", "&amp;J31&amp;", "&amp;K31&amp;", "&amp;L31</f>
-        <v>1204, 1566, 1204, 964, 1204, 2409, 1204, 1204, 973</v>
+        <v>1204, 1566, 1807, 964, 964, 2409, 602, 843, 973</v>
       </c>
       <c r="O31" s="10" t="str">
         <f>"word calibration"&amp;C31&amp;"PosArray[9] = {"&amp;N31&amp;"};"</f>
-        <v>word calibrationSecondPosArray[9] = {1204, 1566, 1204, 964, 1204, 2409, 1204, 1204, 973};</v>
-      </c>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.2">
+        <v>word calibrationSecondPosArray[9] = {1204, 1566, 1807, 964, 964, 2409, 602, 843, 973};</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15">
       <c r="C32" s="11" t="s">
         <v>88</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:12">
       <c r="C33" s="11" t="s">
         <v>89</v>
       </c>
@@ -1455,7 +1455,7 @@
       </c>
       <c r="F33" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>4B4</v>
+        <v>70F</v>
       </c>
       <c r="G33" s="18" t="str">
         <f t="shared" si="14"/>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="H33" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>4B4</v>
+        <v>3C4</v>
       </c>
       <c r="I33" s="18" t="str">
         <f t="shared" si="14"/>
@@ -1471,15 +1471,32 @@
       </c>
       <c r="J33" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>4B4</v>
+        <v>25A</v>
       </c>
       <c r="K33" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>4B4</v>
+        <v>34B</v>
       </c>
       <c r="L33" s="18" t="str">
         <f t="shared" ref="L33" si="15">DEC2HEX(ROUND(L29/10,0))</f>
         <v>3CD</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12">
+      <c r="E39">
+        <v>10</v>
+      </c>
+      <c r="F39">
+        <f>E39*F40/E40</f>
+        <v>0.83028083028083033</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12">
+      <c r="E40">
+        <v>4095</v>
+      </c>
+      <c r="F40">
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -1494,33 +1511,33 @@
   <dimension ref="A2:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.08984375" style="3" customWidth="1"/>
     <col min="2" max="2" width="9" style="3"/>
-    <col min="3" max="3" width="49.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="26.875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.75" style="3" customWidth="1"/>
-    <col min="11" max="11" width="17.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="11.375" style="3" customWidth="1"/>
-    <col min="16" max="16" width="17.75" style="3" customWidth="1"/>
-    <col min="17" max="17" width="16.75" style="3" customWidth="1"/>
-    <col min="18" max="18" width="82.125" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="8.75" style="3"/>
+    <col min="6" max="6" width="7.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.36328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="26.90625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.7265625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="17.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.08984375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.6328125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="11.36328125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="17.7265625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="16.7265625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="82.08984375" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
@@ -1576,7 +1593,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
@@ -1630,7 +1647,7 @@
       </c>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="28">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1674,7 +1691,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1716,7 +1733,7 @@
       </c>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1758,7 +1775,7 @@
       </c>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1800,7 +1817,7 @@
       </c>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1820,7 +1837,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1840,7 +1857,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
         <v>40</v>
@@ -1892,7 +1909,7 @@
       </c>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1934,7 +1951,7 @@
       </c>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1976,7 +1993,7 @@
       </c>
       <c r="R12" s="7"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1996,7 +2013,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="7"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18">
       <c r="A14" s="6"/>
       <c r="B14" s="6" t="s">
         <v>83</v>
@@ -2048,7 +2065,7 @@
       </c>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="28">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -2092,7 +2109,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -2112,7 +2129,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="7"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -2132,7 +2149,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="7"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -2180,7 +2197,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -2216,7 +2233,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -2236,7 +2253,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="7"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18">
       <c r="A21" s="6"/>
       <c r="B21" s="6" t="s">
         <v>51</v>
@@ -2282,7 +2299,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -2318,7 +2335,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>

</xml_diff>

<commit_message>
Update GoodProjectAngel.xlsx for Angle mode configuration
</commit_message>
<xml_diff>
--- a/020_System/40_Design/GoodProjectAngel.xlsx
+++ b/020_System/40_Design/GoodProjectAngel.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\00_Workspace\00_YTP_GoodProject\020_System\40_Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ytben\Desktop\Workspace\MyProject\YTP_GoodProject\020_System\40_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE6EA53-DC6E-4822-92A6-9BD1D4E5D9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19280" windowHeight="6980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,12 +34,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{D319BB4B-6548-4B87-BF5D-8AFBC5844F60}">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -57,52 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="90">
-  <si>
-    <t>Step1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mode1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mode2</t>
-  </si>
-  <si>
-    <t>Mode3</t>
-  </si>
-  <si>
-    <t>Mode4</t>
-  </si>
-  <si>
-    <t>Mode5</t>
-  </si>
-  <si>
-    <t>Mode6</t>
-  </si>
-  <si>
-    <t>Mode7</t>
-  </si>
-  <si>
-    <t>Mode8</t>
-  </si>
-  <si>
-    <t>ValueStep1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ValueStep2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="91">
   <si>
     <t>Unsigned</t>
   </si>
@@ -362,13 +317,55 @@
   <si>
     <t>Second</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>度数</t>
+  </si>
+  <si>
+    <t>数值</t>
+  </si>
+  <si>
+    <t>Signal</t>
+  </si>
+  <si>
+    <t>0x00;Reserved</t>
+  </si>
+  <si>
+    <t>0x01: Mode 4/5/6</t>
+  </si>
+  <si>
+    <t>0x02: Mode 1</t>
+  </si>
+  <si>
+    <t>0x03: Mode 2/7/8</t>
+  </si>
+  <si>
+    <t>0x04: Mode 3</t>
+  </si>
+  <si>
+    <t>0x05: Filling mode</t>
+  </si>
+  <si>
+    <t>0x06;Reserved</t>
+  </si>
+  <si>
+    <t>0x07;Reserved</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,14 +416,21 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,18 +463,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -478,6 +470,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -521,7 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="1" borderId="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -546,33 +544,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="PIDs" xfId="1" xr:uid="{A966D7FC-5586-4BC6-B479-724B0B0D4204}"/>
+    <cellStyle name="PIDs" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -847,667 +866,600 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A6:O40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.7265625" customWidth="1"/>
     <col min="15" max="15" width="77.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:15">
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="3" spans="3:15">
+      <c r="C3" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="15">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" t="s">
+      <c r="F3" s="15">
         <v>2</v>
       </c>
-      <c r="B7">
-        <v>100</v>
-      </c>
-      <c r="C7">
-        <v>20</v>
-      </c>
-      <c r="D7">
-        <f>ROUND(40950*B7/340,0)</f>
-        <v>12044</v>
-      </c>
-      <c r="E7">
-        <f>ROUND(40950*C7/340,0)</f>
-        <v>2409</v>
-      </c>
-      <c r="G7" t="str">
-        <f>"  {" &amp; D7 &amp; ", " &amp; E7 &amp;"},  /* First step is " &amp; B7 &amp; " Second step is " &amp;C7 &amp; " */"</f>
-        <v xml:space="preserve">  {12044, 2409},  /* First step is 100 Second step is 20 */</v>
-      </c>
-      <c r="N7">
-        <v>340</v>
-      </c>
-      <c r="O7">
-        <v>40950</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" t="s">
+      <c r="G3" s="15">
         <v>3</v>
       </c>
-      <c r="B8">
-        <v>300</v>
-      </c>
-      <c r="C8">
-        <v>30</v>
-      </c>
-      <c r="D8">
-        <f t="shared" ref="D8:D14" si="0">ROUND(40950*B8/340,0)</f>
-        <v>36132</v>
-      </c>
-      <c r="E8">
-        <f t="shared" ref="E8:E14" si="1">ROUND(40950*C8/340,0)</f>
-        <v>3613</v>
-      </c>
-      <c r="G8" t="str">
-        <f t="shared" ref="G8:G14" si="2">"  {" &amp; D8 &amp; ", " &amp; E8 &amp;"},  /* First step is " &amp; B8 &amp; " Second step is " &amp;C8 &amp; " */"</f>
-        <v xml:space="preserve">  {36132, 3613},  /* First step is 300 Second step is 30 */</v>
-      </c>
-      <c r="N8">
-        <v>360</v>
-      </c>
-      <c r="O8">
-        <f>N8*O7/N7</f>
-        <v>43358.823529411762</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" t="s">
+      <c r="H3" s="15">
         <v>4</v>
       </c>
-      <c r="B9">
-        <v>200</v>
-      </c>
-      <c r="C9">
-        <v>50</v>
-      </c>
-      <c r="D9">
+      <c r="I3" s="15">
+        <v>5</v>
+      </c>
+      <c r="J3" s="15">
+        <v>6</v>
+      </c>
+      <c r="K3" s="15">
+        <v>7</v>
+      </c>
+      <c r="L3" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" ht="18.5">
+      <c r="C4" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" ht="18.5">
+      <c r="C5" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0</v>
+      </c>
+      <c r="E5" s="16">
+        <v>247</v>
+      </c>
+      <c r="F5" s="16">
+        <v>337</v>
+      </c>
+      <c r="G5" s="16">
+        <v>67</v>
+      </c>
+      <c r="H5" s="16">
+        <v>292</v>
+      </c>
+      <c r="I5" s="16">
+        <v>44.5</v>
+      </c>
+      <c r="J5" s="16">
+        <v>0</v>
+      </c>
+      <c r="K5" s="16">
+        <v>0</v>
+      </c>
+      <c r="L5" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" ht="18.5">
+      <c r="C6" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16">
+        <v>327</v>
+      </c>
+      <c r="F6" s="16">
+        <v>237</v>
+      </c>
+      <c r="G6" s="16">
+        <v>237</v>
+      </c>
+      <c r="H6" s="16">
+        <v>57</v>
+      </c>
+      <c r="I6" s="16">
+        <v>34.5</v>
+      </c>
+      <c r="J6" s="16">
+        <v>0</v>
+      </c>
+      <c r="K6" s="16">
+        <v>0</v>
+      </c>
+      <c r="L6" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15">
+      <c r="C7" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="12">
+        <f>ROUND(40950*D5/340,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="12">
+        <f t="shared" ref="E7:K8" si="0">ROUND(40950*E5/340,0)</f>
+        <v>29749</v>
+      </c>
+      <c r="F7" s="12">
         <f t="shared" si="0"/>
-        <v>24088</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>6022</v>
-      </c>
-      <c r="G9" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  {24088, 6022},  /* First step is 200 Second step is 50 */</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>110</v>
-      </c>
-      <c r="C10">
+        <v>40589</v>
+      </c>
+      <c r="G7" s="12">
+        <f t="shared" si="0"/>
+        <v>8070</v>
+      </c>
+      <c r="H7" s="12">
+        <f t="shared" si="0"/>
+        <v>35169</v>
+      </c>
+      <c r="I7" s="12">
+        <f t="shared" si="0"/>
+        <v>5360</v>
+      </c>
+      <c r="J7" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="12">
+        <f t="shared" ref="L7" si="1">ROUND(40950*L5/340,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15">
+      <c r="C8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="12">
+        <f>ROUND(40950*D6/340,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="12">
+        <f t="shared" si="0"/>
+        <v>39384</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="0"/>
+        <v>28545</v>
+      </c>
+      <c r="G8" s="12">
+        <f t="shared" si="0"/>
+        <v>28545</v>
+      </c>
+      <c r="H8" s="12">
+        <f t="shared" si="0"/>
+        <v>6865</v>
+      </c>
+      <c r="I8" s="12">
+        <f t="shared" si="0"/>
+        <v>4155</v>
+      </c>
+      <c r="J8" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <f t="shared" ref="L8" si="2">ROUND(40950*L6/340,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" ht="18.5">
+      <c r="C9" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="13">
+        <f>IF(D$4="Yes",ROUND(D7/10,0),65535)</f>
+        <v>65535</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" ref="E9:L10" si="3">IF(E$4="Yes",ROUND(E7/10,0),65535)</f>
+        <v>2975</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="3"/>
+        <v>4059</v>
+      </c>
+      <c r="G9" s="13">
+        <f t="shared" si="3"/>
+        <v>807</v>
+      </c>
+      <c r="H9" s="13">
+        <f t="shared" si="3"/>
+        <v>3517</v>
+      </c>
+      <c r="I9" s="13">
+        <f t="shared" si="3"/>
+        <v>536</v>
+      </c>
+      <c r="J9" s="13">
+        <f t="shared" si="3"/>
+        <v>65535</v>
+      </c>
+      <c r="K9" s="13">
+        <f t="shared" si="3"/>
+        <v>65535</v>
+      </c>
+      <c r="L9" s="13">
+        <f t="shared" si="3"/>
+        <v>65535</v>
+      </c>
+      <c r="N9" t="str">
+        <f>D9&amp;", "&amp;E9&amp;", "&amp;F9&amp;", "&amp;G9&amp;", "&amp;H9&amp;", "&amp;I9&amp;", "&amp;J9&amp;", "&amp;K9&amp;", "&amp;L9</f>
+        <v>65535, 2975, 4059, 807, 3517, 536, 65535, 65535, 65535</v>
+      </c>
+      <c r="O9" s="10" t="str">
+        <f>"word calibration"&amp;C9&amp;"PosArray[9] = {"&amp;N9&amp;"};"</f>
+        <v>word calibrationFirstPosArray[9] = {65535, 2975, 4059, 807, 3517, 536, 65535, 65535, 65535};</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" ht="18.5">
+      <c r="C10" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="13">
+        <f>IF(D$4="Yes",ROUND(D8/10,0),65535)</f>
+        <v>65535</v>
+      </c>
+      <c r="E10" s="13">
+        <f t="shared" si="3"/>
+        <v>3938</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="3"/>
+        <v>2855</v>
+      </c>
+      <c r="G10" s="13">
+        <f t="shared" si="3"/>
+        <v>2855</v>
+      </c>
+      <c r="H10" s="13">
+        <f t="shared" si="3"/>
+        <v>687</v>
+      </c>
+      <c r="I10" s="13">
+        <f t="shared" si="3"/>
+        <v>416</v>
+      </c>
+      <c r="J10" s="13">
+        <f t="shared" si="3"/>
+        <v>65535</v>
+      </c>
+      <c r="K10" s="13">
+        <f t="shared" si="3"/>
+        <v>65535</v>
+      </c>
+      <c r="L10" s="13">
+        <f t="shared" si="3"/>
+        <v>65535</v>
+      </c>
+      <c r="N10" t="str">
+        <f>D10&amp;", "&amp;E10&amp;", "&amp;F10&amp;", "&amp;G10&amp;", "&amp;H10&amp;", "&amp;I10&amp;", "&amp;J10&amp;", "&amp;K10&amp;", "&amp;L10</f>
+        <v>65535, 3938, 2855, 2855, 687, 416, 65535, 65535, 65535</v>
+      </c>
+      <c r="O10" s="10" t="str">
+        <f>"word calibration"&amp;C10&amp;"PosArray[9] = {"&amp;N10&amp;"};"</f>
+        <v>word calibrationSecondPosArray[9] = {65535, 3938, 2855, 2855, 687, 416, 65535, 65535, 65535};</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15">
+      <c r="C11" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="14" t="str">
+        <f>DEC2HEX(D9)</f>
+        <v>FFFF</v>
+      </c>
+      <c r="E11" s="14" t="str">
+        <f t="shared" ref="E11:L12" si="4">DEC2HEX(E9)</f>
+        <v>B9F</v>
+      </c>
+      <c r="F11" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>FDB</v>
+      </c>
+      <c r="G11" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>327</v>
+      </c>
+      <c r="H11" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>DBD</v>
+      </c>
+      <c r="I11" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>218</v>
+      </c>
+      <c r="J11" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFF</v>
+      </c>
+      <c r="K11" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFF</v>
+      </c>
+      <c r="L11" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFF</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15">
+      <c r="C12" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="14" t="str">
+        <f>DEC2HEX(D10)</f>
+        <v>FFFF</v>
+      </c>
+      <c r="E12" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>F62</v>
+      </c>
+      <c r="F12" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>B27</v>
+      </c>
+      <c r="G12" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>B27</v>
+      </c>
+      <c r="H12" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>2AF</v>
+      </c>
+      <c r="I12" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>1A0</v>
+      </c>
+      <c r="J12" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFF</v>
+      </c>
+      <c r="K12" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFF</v>
+      </c>
+      <c r="L12" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFF</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10">
+      <c r="E17" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>13249</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>9635</v>
-      </c>
-      <c r="G10" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  {13249, 9635},  /* First step is 110 Second step is 80 */</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11">
-        <v>320</v>
-      </c>
-      <c r="C11">
-        <v>250</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>38541</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>30110</v>
-      </c>
-      <c r="G11" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  {38541, 30110},  /* First step is 320 Second step is 250 */</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>320</v>
-      </c>
-      <c r="C12">
-        <v>50</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>38541</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>6022</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  {38541, 6022},  /* First step is 320 Second step is 50 */</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>270</v>
-      </c>
-      <c r="C13">
-        <v>180</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>32519</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>21679</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  {32519, 21679},  /* First step is 270 Second step is 180 */</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14">
-        <v>200</v>
-      </c>
-      <c r="C14">
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>24088</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>9635</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  {24088, 9635},  /* First step is 200 Second step is 80 */</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="C16">
-        <v>100</v>
-      </c>
-      <c r="D16">
-        <f>ROUND(40950*C16/340,0)</f>
-        <v>12044</v>
-      </c>
-      <c r="E16">
-        <f>ROUND(D16/10,0)</f>
-        <v>1204</v>
-      </c>
-      <c r="F16" t="str">
-        <f>DEC2HEX(ROUND(D16/10,0))</f>
-        <v>4B4</v>
-      </c>
-    </row>
-    <row r="17" spans="3:15">
-      <c r="C17">
-        <v>180</v>
-      </c>
-      <c r="D17">
-        <f t="shared" ref="D17:D18" si="3">ROUND(40950*C17/340,0)</f>
-        <v>21679</v>
-      </c>
-      <c r="E17">
-        <f t="shared" ref="E17:E18" si="4">ROUND(D17/10,0)</f>
-        <v>2168</v>
-      </c>
-      <c r="F17" t="str">
-        <f t="shared" ref="F17:F18" si="5">DEC2HEX(ROUND(D17/10,0))</f>
-        <v>878</v>
-      </c>
-    </row>
-    <row r="18" spans="3:15">
-      <c r="C18">
-        <v>460</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="3"/>
-        <v>55403</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="4"/>
-        <v>5540</v>
-      </c>
-      <c r="F18" t="str">
+    </row>
+    <row r="18" spans="3:10">
+      <c r="E18" s="20">
+        <v>3000</v>
+      </c>
+      <c r="F18" s="18">
+        <f>E18*340/4095</f>
+        <v>249.08424908424908</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="18">
+        <f>4095*J18/340</f>
+        <v>3962.5147058823532</v>
+      </c>
+      <c r="J18" s="19">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10">
+      <c r="E19" s="20">
+        <v>3001</v>
+      </c>
+      <c r="F19" s="18">
+        <f t="shared" ref="F19:F24" si="5">E19*340/4095</f>
+        <v>249.16727716727718</v>
+      </c>
+      <c r="I19" s="18">
+        <f t="shared" ref="I19:I24" si="6">4095*J19/340</f>
+        <v>3950.4705882352941</v>
+      </c>
+      <c r="J19" s="19">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10">
+      <c r="E20" s="20">
+        <v>3002</v>
+      </c>
+      <c r="F20" s="18">
         <f t="shared" si="5"/>
-        <v>15A4</v>
-      </c>
-    </row>
-    <row r="25" spans="3:15">
-      <c r="C25" s="11"/>
-      <c r="D25" s="12">
-        <v>0</v>
-      </c>
-      <c r="E25" s="12">
-        <v>1</v>
-      </c>
-      <c r="F25" s="12">
-        <v>2</v>
-      </c>
-      <c r="G25" s="12">
-        <v>3</v>
-      </c>
-      <c r="H25" s="12">
-        <v>4</v>
-      </c>
-      <c r="I25" s="12">
-        <v>5</v>
-      </c>
-      <c r="J25" s="12">
-        <v>6</v>
-      </c>
-      <c r="K25" s="12">
-        <v>7</v>
-      </c>
-      <c r="L25" s="12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="3:15" ht="18.5">
-      <c r="C26" s="11" t="s">
+        <v>249.25030525030525</v>
+      </c>
+      <c r="I20" s="18">
+        <f t="shared" si="6"/>
+        <v>3962.5147058823532</v>
+      </c>
+      <c r="J20" s="19">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10">
+      <c r="E21" s="20">
+        <v>3003</v>
+      </c>
+      <c r="F21" s="18">
+        <f t="shared" si="5"/>
+        <v>249.33333333333334</v>
+      </c>
+      <c r="I21" s="18">
+        <f t="shared" si="6"/>
+        <v>3926.3823529411766</v>
+      </c>
+      <c r="J21" s="19">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10">
+      <c r="E22" s="20">
+        <v>3004</v>
+      </c>
+      <c r="F22" s="18">
+        <f t="shared" si="5"/>
+        <v>249.41636141636141</v>
+      </c>
+      <c r="I22" s="18">
+        <f t="shared" si="6"/>
+        <v>3926.3823529411766</v>
+      </c>
+      <c r="J22" s="19">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10">
+      <c r="E23" s="20">
+        <v>3005</v>
+      </c>
+      <c r="F23" s="18">
+        <f t="shared" si="5"/>
+        <v>249.49938949938951</v>
+      </c>
+      <c r="I23" s="18">
+        <f t="shared" si="6"/>
+        <v>3793.8970588235293</v>
+      </c>
+      <c r="J23" s="19">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10">
+      <c r="E24" s="20">
+        <v>3006</v>
+      </c>
+      <c r="F24" s="18">
+        <f t="shared" si="5"/>
+        <v>249.58241758241758</v>
+      </c>
+      <c r="I24" s="18">
+        <f t="shared" si="6"/>
+        <v>4456.3235294117649</v>
+      </c>
+      <c r="J24" s="19">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10">
+      <c r="C27" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10">
+      <c r="C28" s="21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10">
+      <c r="C29" s="21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10">
+      <c r="C30" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10">
+      <c r="C31" s="21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10">
+      <c r="C32" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D26" s="13">
-        <v>200</v>
-      </c>
-      <c r="E26" s="13">
-        <v>230</v>
-      </c>
-      <c r="F26" s="13">
-        <v>200</v>
-      </c>
-      <c r="G26" s="13">
-        <v>80</v>
-      </c>
-      <c r="H26" s="13">
-        <v>230</v>
-      </c>
-      <c r="I26" s="13">
-        <v>250</v>
-      </c>
-      <c r="J26" s="13">
-        <v>200</v>
-      </c>
-      <c r="K26" s="13">
-        <v>150.5</v>
-      </c>
-      <c r="L26" s="13">
-        <v>180.8</v>
-      </c>
-    </row>
-    <row r="27" spans="3:15" ht="18.5">
-      <c r="C27" s="11" t="s">
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="13">
-        <v>100</v>
-      </c>
-      <c r="E27" s="13">
-        <v>130</v>
-      </c>
-      <c r="F27" s="13">
-        <v>150</v>
-      </c>
-      <c r="G27" s="13">
-        <v>80</v>
-      </c>
-      <c r="H27" s="13">
-        <v>80</v>
-      </c>
-      <c r="I27" s="13">
-        <v>200</v>
-      </c>
-      <c r="J27" s="13">
-        <v>50</v>
-      </c>
-      <c r="K27" s="13">
-        <v>70</v>
-      </c>
-      <c r="L27" s="13">
-        <v>80.8</v>
-      </c>
-    </row>
-    <row r="28" spans="3:15">
-      <c r="C28" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" s="14">
-        <f>ROUND(40950*D26/340,0)</f>
-        <v>24088</v>
-      </c>
-      <c r="E28" s="14">
-        <f t="shared" ref="E28:K29" si="6">ROUND(40950*E26/340,0)</f>
-        <v>27701</v>
-      </c>
-      <c r="F28" s="14">
-        <f t="shared" si="6"/>
-        <v>24088</v>
-      </c>
-      <c r="G28" s="14">
-        <f t="shared" si="6"/>
-        <v>9635</v>
-      </c>
-      <c r="H28" s="14">
-        <f t="shared" si="6"/>
-        <v>27701</v>
-      </c>
-      <c r="I28" s="14">
-        <f t="shared" si="6"/>
-        <v>30110</v>
-      </c>
-      <c r="J28" s="14">
-        <f t="shared" si="6"/>
-        <v>24088</v>
-      </c>
-      <c r="K28" s="14">
-        <f t="shared" si="6"/>
-        <v>18126</v>
-      </c>
-      <c r="L28" s="14">
-        <f t="shared" ref="L28" si="7">ROUND(40950*L26/340,0)</f>
-        <v>21776</v>
-      </c>
-    </row>
-    <row r="29" spans="3:15">
-      <c r="C29" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="14">
-        <f>ROUND(40950*D27/340,0)</f>
-        <v>12044</v>
-      </c>
-      <c r="E29" s="14">
-        <f t="shared" si="6"/>
-        <v>15657</v>
-      </c>
-      <c r="F29" s="14">
-        <f t="shared" si="6"/>
-        <v>18066</v>
-      </c>
-      <c r="G29" s="14">
-        <f t="shared" si="6"/>
-        <v>9635</v>
-      </c>
-      <c r="H29" s="14">
-        <f t="shared" si="6"/>
-        <v>9635</v>
-      </c>
-      <c r="I29" s="14">
-        <f t="shared" si="6"/>
-        <v>24088</v>
-      </c>
-      <c r="J29" s="14">
-        <f t="shared" si="6"/>
-        <v>6022</v>
-      </c>
-      <c r="K29" s="14">
-        <f t="shared" si="6"/>
-        <v>8431</v>
-      </c>
-      <c r="L29" s="14">
-        <f t="shared" ref="L29" si="8">ROUND(40950*L27/340,0)</f>
-        <v>9732</v>
-      </c>
-    </row>
-    <row r="30" spans="3:15" ht="18.5">
-      <c r="C30" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D30" s="15">
-        <f>ROUND(D28/10,0)</f>
-        <v>2409</v>
-      </c>
-      <c r="E30" s="15">
-        <f t="shared" ref="E30:K31" si="9">ROUND(E28/10,0)</f>
-        <v>2770</v>
-      </c>
-      <c r="F30" s="15">
-        <f t="shared" si="9"/>
-        <v>2409</v>
-      </c>
-      <c r="G30" s="15">
-        <f t="shared" si="9"/>
-        <v>964</v>
-      </c>
-      <c r="H30" s="15">
-        <f t="shared" si="9"/>
-        <v>2770</v>
-      </c>
-      <c r="I30" s="15">
-        <f t="shared" si="9"/>
-        <v>3011</v>
-      </c>
-      <c r="J30" s="15">
-        <f t="shared" si="9"/>
-        <v>2409</v>
-      </c>
-      <c r="K30" s="15">
-        <f t="shared" si="9"/>
-        <v>1813</v>
-      </c>
-      <c r="L30" s="15">
-        <f t="shared" ref="L30" si="10">ROUND(L28/10,0)</f>
-        <v>2178</v>
-      </c>
-      <c r="N30" t="str">
-        <f>D30&amp;", "&amp;E30&amp;", "&amp;F30&amp;", "&amp;G30&amp;", "&amp;H30&amp;", "&amp;I30&amp;", "&amp;J30&amp;", "&amp;K30&amp;", "&amp;L30</f>
-        <v>2409, 2770, 2409, 964, 2770, 3011, 2409, 1813, 2178</v>
-      </c>
-      <c r="O30" s="10" t="str">
-        <f>"word calibration"&amp;C30&amp;"PosArray[9] = {"&amp;N30&amp;"};"</f>
-        <v>word calibrationFirstPosArray[9] = {2409, 2770, 2409, 964, 2770, 3011, 2409, 1813, 2178};</v>
-      </c>
-    </row>
-    <row r="31" spans="3:15" ht="18.5">
-      <c r="C31" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="16">
-        <f>ROUND(D29/10,0)</f>
-        <v>1204</v>
-      </c>
-      <c r="E31" s="16">
-        <f t="shared" si="9"/>
-        <v>1566</v>
-      </c>
-      <c r="F31" s="16">
-        <f t="shared" si="9"/>
-        <v>1807</v>
-      </c>
-      <c r="G31" s="16">
-        <f t="shared" si="9"/>
-        <v>964</v>
-      </c>
-      <c r="H31" s="16">
-        <f t="shared" si="9"/>
-        <v>964</v>
-      </c>
-      <c r="I31" s="16">
-        <f t="shared" si="9"/>
-        <v>2409</v>
-      </c>
-      <c r="J31" s="16">
-        <f t="shared" si="9"/>
-        <v>602</v>
-      </c>
-      <c r="K31" s="16">
-        <f t="shared" si="9"/>
-        <v>843</v>
-      </c>
-      <c r="L31" s="16">
-        <f t="shared" ref="L31" si="11">ROUND(L29/10,0)</f>
-        <v>973</v>
-      </c>
-      <c r="N31" t="str">
-        <f>D31&amp;", "&amp;E31&amp;", "&amp;F31&amp;", "&amp;G31&amp;", "&amp;H31&amp;", "&amp;I31&amp;", "&amp;J31&amp;", "&amp;K31&amp;", "&amp;L31</f>
-        <v>1204, 1566, 1807, 964, 964, 2409, 602, 843, 973</v>
-      </c>
-      <c r="O31" s="10" t="str">
-        <f>"word calibration"&amp;C31&amp;"PosArray[9] = {"&amp;N31&amp;"};"</f>
-        <v>word calibrationSecondPosArray[9] = {1204, 1566, 1807, 964, 964, 2409, 602, 843, 973};</v>
-      </c>
-    </row>
-    <row r="32" spans="3:15">
-      <c r="C32" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D32" s="17" t="str">
-        <f>DEC2HEX(ROUND(D28/10,0))</f>
-        <v>969</v>
-      </c>
-      <c r="E32" s="17" t="str">
-        <f t="shared" ref="E32:K32" si="12">DEC2HEX(ROUND(E28/10,0))</f>
-        <v>AD2</v>
-      </c>
-      <c r="F32" s="17" t="str">
-        <f t="shared" si="12"/>
-        <v>969</v>
-      </c>
-      <c r="G32" s="17" t="str">
-        <f t="shared" si="12"/>
-        <v>3C4</v>
-      </c>
-      <c r="H32" s="17" t="str">
-        <f t="shared" si="12"/>
-        <v>AD2</v>
-      </c>
-      <c r="I32" s="17" t="str">
-        <f t="shared" si="12"/>
-        <v>BC3</v>
-      </c>
-      <c r="J32" s="17" t="str">
-        <f t="shared" si="12"/>
-        <v>969</v>
-      </c>
-      <c r="K32" s="17" t="str">
-        <f t="shared" si="12"/>
-        <v>715</v>
-      </c>
-      <c r="L32" s="17" t="str">
-        <f t="shared" ref="L32" si="13">DEC2HEX(ROUND(L28/10,0))</f>
-        <v>882</v>
-      </c>
-    </row>
-    <row r="33" spans="3:12">
-      <c r="C33" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D33" s="18" t="str">
-        <f>DEC2HEX(ROUND(D29/10,0))</f>
-        <v>4B4</v>
-      </c>
-      <c r="E33" s="18" t="str">
-        <f t="shared" ref="E33:K33" si="14">DEC2HEX(ROUND(E29/10,0))</f>
-        <v>61E</v>
-      </c>
-      <c r="F33" s="18" t="str">
-        <f t="shared" si="14"/>
-        <v>70F</v>
-      </c>
-      <c r="G33" s="18" t="str">
-        <f t="shared" si="14"/>
-        <v>3C4</v>
-      </c>
-      <c r="H33" s="18" t="str">
-        <f t="shared" si="14"/>
-        <v>3C4</v>
-      </c>
-      <c r="I33" s="18" t="str">
-        <f t="shared" si="14"/>
-        <v>969</v>
-      </c>
-      <c r="J33" s="18" t="str">
-        <f t="shared" si="14"/>
-        <v>25A</v>
-      </c>
-      <c r="K33" s="18" t="str">
-        <f t="shared" si="14"/>
-        <v>34B</v>
-      </c>
-      <c r="L33" s="18" t="str">
-        <f t="shared" ref="L33" si="15">DEC2HEX(ROUND(L29/10,0))</f>
-        <v>3CD</v>
-      </c>
-    </row>
-    <row r="39" spans="3:12">
-      <c r="E39">
-        <v>10</v>
-      </c>
-      <c r="F39">
-        <f>E39*F40/E40</f>
-        <v>0.83028083028083033</v>
-      </c>
-    </row>
-    <row r="40" spans="3:12">
-      <c r="E40">
-        <v>4095</v>
-      </c>
-      <c r="F40">
-        <v>340</v>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="21" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="D4:L6">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>D$4="Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:L4">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFDF32A-9B3A-4F81-AD96-0784476499BF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1516,119 +1468,119 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" style="3" customWidth="1"/>
     <col min="2" max="2" width="9" style="3"/>
-    <col min="3" max="3" width="49.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.36328125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="26.90625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.453125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="26.81640625" style="3" customWidth="1"/>
     <col min="10" max="10" width="12.7265625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="17.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.08984375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.6328125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="11.36328125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="12.1796875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.54296875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="11.453125" style="3" customWidth="1"/>
     <col min="16" max="16" width="17.7265625" style="3" customWidth="1"/>
     <col min="17" max="17" width="16.7265625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="82.08984375" style="3" customWidth="1"/>
+    <col min="18" max="18" width="82.1796875" style="3" customWidth="1"/>
     <col min="19" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:18">
       <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="O2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="P2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="6" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="K3" s="1">
         <v>0</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="M3" s="1">
         <v>1</v>
@@ -1637,13 +1589,13 @@
         <v>0</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="R3" s="7"/>
     </row>
@@ -1655,22 +1607,22 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="M4" s="1">
         <v>1</v>
@@ -1679,16 +1631,16 @@
         <v>0</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -1699,22 +1651,22 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="M5" s="1">
         <v>1</v>
@@ -1723,13 +1675,13 @@
         <v>0</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="R5" s="7"/>
     </row>
@@ -1741,22 +1693,22 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="K6" s="1">
         <v>0</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="M6" s="1">
         <v>1</v>
@@ -1765,13 +1717,13 @@
         <v>0</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="R6" s="7"/>
     </row>
@@ -1783,22 +1735,22 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="K7" s="1">
         <v>0</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="M7" s="1">
         <v>1</v>
@@ -1807,13 +1759,13 @@
         <v>0</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="R7" s="7"/>
     </row>
@@ -1860,37 +1812,37 @@
     <row r="10" spans="1:18">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="M10" s="1">
         <v>1</v>
@@ -1899,13 +1851,13 @@
         <v>0</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="R10" s="7"/>
     </row>
@@ -1920,19 +1872,19 @@
         <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="K11" s="1">
         <v>0</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="M11" s="1">
         <v>1</v>
@@ -1941,13 +1893,13 @@
         <v>0</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="R11" s="7"/>
     </row>
@@ -1959,22 +1911,22 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="K12" s="1">
         <v>0</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="M12" s="1">
         <v>1</v>
@@ -1983,13 +1935,13 @@
         <v>0</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="R12" s="7"/>
     </row>
@@ -2016,37 +1968,37 @@
     <row r="14" spans="1:18">
       <c r="A14" s="6"/>
       <c r="B14" s="6" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="G14" s="1">
         <v>0</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="K14" s="1">
         <v>0</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="M14" s="1">
         <v>1</v>
@@ -2055,13 +2007,13 @@
         <v>0</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="R14" s="7"/>
     </row>
@@ -2076,19 +2028,19 @@
         <v>1</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="M15" s="1">
         <v>1</v>
@@ -2097,16 +2049,16 @@
         <v>0</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="R15" s="9" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -2151,50 +2103,50 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="6" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="F18" s="1">
         <v>18</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="R18" s="9" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -2205,32 +2157,32 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="R19" s="7" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -2256,47 +2208,47 @@
     <row r="21" spans="1:18">
       <c r="A21" s="6"/>
       <c r="B21" s="6" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="F21" s="1">
         <v>18</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="L21" s="8"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="R21" s="9" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -2307,32 +2259,32 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="L22" s="8"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="R22" s="7" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -2360,4 +2312,97 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D7:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="7" spans="4:8">
+      <c r="D7">
+        <v>243</v>
+      </c>
+      <c r="E7">
+        <v>333</v>
+      </c>
+      <c r="F7">
+        <v>288</v>
+      </c>
+      <c r="G7">
+        <v>63</v>
+      </c>
+      <c r="H7">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8">
+      <c r="D8">
+        <v>323</v>
+      </c>
+      <c r="E8">
+        <v>233</v>
+      </c>
+      <c r="F8">
+        <v>53</v>
+      </c>
+      <c r="G8">
+        <v>233</v>
+      </c>
+      <c r="H8">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8">
+      <c r="D9">
+        <f>D7+4</f>
+        <v>247</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9:H10" si="0">E7+4</f>
+        <v>337</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>44.5</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8">
+      <c r="D10">
+        <f>D8+4</f>
+        <v>327</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>237</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>237</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>34.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Release 1.5 1. Add double and signal valve control 2. Add double valve cycle test 3. Add configuration for Signal, Double, Double Test config, by cal message 4. Fix issue can't receive LIN message after receive LIN error frame
</commit_message>
<xml_diff>
--- a/020_System/40_Design/GoodProjectAngel.xlsx
+++ b/020_System/40_Design/GoodProjectAngel.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ytben\Desktop\Workspace\MyProject\YTP_GoodProject\020_System\40_Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\050_Workspace\010_YTP_SENT\020_System\40_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BA0613-BC4E-4E23-B5B3-0709B1FAC65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19280" windowHeight="6980"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,12 +35,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="112">
   <si>
     <t>Unsigned</t>
   </si>
@@ -359,23 +360,104 @@
   </si>
   <si>
     <t>0x07;Reserved</t>
+  </si>
+  <si>
+    <t>0x22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstPos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SecondPos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ValveType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01: SignalValve
+0x02: DoubleValve
+0xA1: SignalValveTest
+0xA2: DoubleValveTest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
+    <t>Data5</t>
+  </si>
+  <si>
+    <t>Data6</t>
+  </si>
+  <si>
+    <t>Data7</t>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Message Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Master_Cal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yt_Cal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01: CalModePosition
+0xAA: CalModeType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -408,7 +490,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -416,7 +498,7 @@
     <font>
       <b/>
       <sz val="14"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -425,7 +507,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -519,7 +601,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="1" borderId="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -575,10 +657,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="PIDs" xfId="1"/>
+    <cellStyle name="PIDs" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -866,22 +952,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7265625" customWidth="1"/>
-    <col min="15" max="15" width="77.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.75" customWidth="1"/>
+    <col min="15" max="15" width="77.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:15">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C3" s="11" t="s">
         <v>82</v>
       </c>
@@ -913,12 +999,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="3:15" ht="18.5">
+    <row r="4" spans="3:15" ht="18" x14ac:dyDescent="0.25">
       <c r="C4" s="11" t="s">
         <v>77</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>79</v>
@@ -945,15 +1031,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="3:15" ht="18.5">
+    <row r="5" spans="3:15" ht="18" x14ac:dyDescent="0.25">
       <c r="C5" s="11" t="s">
         <v>75</v>
       </c>
       <c r="D5" s="16">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="E5" s="16">
-        <v>247</v>
+        <v>300</v>
       </c>
       <c r="F5" s="16">
         <v>337</v>
@@ -977,15 +1063,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="3:15" ht="18.5">
+    <row r="6" spans="3:15" ht="18" x14ac:dyDescent="0.25">
       <c r="C6" s="11" t="s">
         <v>76</v>
       </c>
       <c r="D6" s="16">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="E6" s="16">
-        <v>327</v>
+        <v>270</v>
       </c>
       <c r="F6" s="16">
         <v>237</v>
@@ -1009,17 +1095,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:15">
+    <row r="7" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C7" s="11" t="s">
         <v>75</v>
       </c>
       <c r="D7" s="12">
         <f>ROUND(40950*D5/340,0)</f>
-        <v>0</v>
+        <v>39746</v>
       </c>
       <c r="E7" s="12">
         <f t="shared" ref="E7:K8" si="0">ROUND(40950*E5/340,0)</f>
-        <v>29749</v>
+        <v>36132</v>
       </c>
       <c r="F7" s="12">
         <f t="shared" si="0"/>
@@ -1050,17 +1136,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:15">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C8" s="11" t="s">
         <v>76</v>
       </c>
       <c r="D8" s="12">
         <f>ROUND(40950*D6/340,0)</f>
-        <v>0</v>
+        <v>32519</v>
       </c>
       <c r="E8" s="12">
         <f t="shared" si="0"/>
-        <v>39384</v>
+        <v>32519</v>
       </c>
       <c r="F8" s="12">
         <f t="shared" si="0"/>
@@ -1091,17 +1177,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="3:15" ht="18.5">
+    <row r="9" spans="3:15" ht="18" x14ac:dyDescent="0.25">
       <c r="C9" s="11" t="s">
         <v>75</v>
       </c>
       <c r="D9" s="13">
         <f>IF(D$4="Yes",ROUND(D7/10,0),65535)</f>
-        <v>65535</v>
+        <v>3975</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" ref="E9:L10" si="3">IF(E$4="Yes",ROUND(E7/10,0),65535)</f>
-        <v>2975</v>
+        <v>3613</v>
       </c>
       <c r="F9" s="13">
         <f t="shared" si="3"/>
@@ -1133,24 +1219,24 @@
       </c>
       <c r="N9" t="str">
         <f>D9&amp;", "&amp;E9&amp;", "&amp;F9&amp;", "&amp;G9&amp;", "&amp;H9&amp;", "&amp;I9&amp;", "&amp;J9&amp;", "&amp;K9&amp;", "&amp;L9</f>
-        <v>65535, 2975, 4059, 807, 3517, 536, 65535, 65535, 65535</v>
+        <v>3975, 3613, 4059, 807, 3517, 536, 65535, 65535, 65535</v>
       </c>
       <c r="O9" s="10" t="str">
         <f>"word calibration"&amp;C9&amp;"PosArray[9] = {"&amp;N9&amp;"};"</f>
-        <v>word calibrationFirstPosArray[9] = {65535, 2975, 4059, 807, 3517, 536, 65535, 65535, 65535};</v>
-      </c>
-    </row>
-    <row r="10" spans="3:15" ht="18.5">
+        <v>word calibrationFirstPosArray[9] = {3975, 3613, 4059, 807, 3517, 536, 65535, 65535, 65535};</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" ht="18" x14ac:dyDescent="0.25">
       <c r="C10" s="11" t="s">
         <v>76</v>
       </c>
       <c r="D10" s="13">
         <f>IF(D$4="Yes",ROUND(D8/10,0),65535)</f>
-        <v>65535</v>
+        <v>3252</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" si="3"/>
-        <v>3938</v>
+        <v>3252</v>
       </c>
       <c r="F10" s="13">
         <f t="shared" si="3"/>
@@ -1182,24 +1268,24 @@
       </c>
       <c r="N10" t="str">
         <f>D10&amp;", "&amp;E10&amp;", "&amp;F10&amp;", "&amp;G10&amp;", "&amp;H10&amp;", "&amp;I10&amp;", "&amp;J10&amp;", "&amp;K10&amp;", "&amp;L10</f>
-        <v>65535, 3938, 2855, 2855, 687, 416, 65535, 65535, 65535</v>
+        <v>3252, 3252, 2855, 2855, 687, 416, 65535, 65535, 65535</v>
       </c>
       <c r="O10" s="10" t="str">
         <f>"word calibration"&amp;C10&amp;"PosArray[9] = {"&amp;N10&amp;"};"</f>
-        <v>word calibrationSecondPosArray[9] = {65535, 3938, 2855, 2855, 687, 416, 65535, 65535, 65535};</v>
-      </c>
-    </row>
-    <row r="11" spans="3:15">
+        <v>word calibrationSecondPosArray[9] = {3252, 3252, 2855, 2855, 687, 416, 65535, 65535, 65535};</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C11" s="11" t="s">
         <v>75</v>
       </c>
       <c r="D11" s="14" t="str">
         <f>DEC2HEX(D9)</f>
-        <v>FFFF</v>
+        <v>F87</v>
       </c>
       <c r="E11" s="14" t="str">
         <f t="shared" ref="E11:L12" si="4">DEC2HEX(E9)</f>
-        <v>B9F</v>
+        <v>E1D</v>
       </c>
       <c r="F11" s="14" t="str">
         <f t="shared" si="4"/>
@@ -1230,17 +1316,17 @@
         <v>FFFF</v>
       </c>
     </row>
-    <row r="12" spans="3:15">
+    <row r="12" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C12" s="11" t="s">
         <v>76</v>
       </c>
       <c r="D12" s="14" t="str">
         <f>DEC2HEX(D10)</f>
-        <v>FFFF</v>
+        <v>CB4</v>
       </c>
       <c r="E12" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>F62</v>
+        <v>CB4</v>
       </c>
       <c r="F12" s="14" t="str">
         <f t="shared" si="4"/>
@@ -1271,7 +1357,7 @@
         <v>FFFF</v>
       </c>
     </row>
-    <row r="17" spans="3:10">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E17" s="12" t="s">
         <v>81</v>
       </c>
@@ -1287,7 +1373,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="3:10">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E18" s="20">
         <v>3000</v>
       </c>
@@ -1305,7 +1391,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="19" spans="3:10">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E19" s="20">
         <v>3001</v>
       </c>
@@ -1321,7 +1407,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="20" spans="3:10">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E20" s="20">
         <v>3002</v>
       </c>
@@ -1337,7 +1423,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="21" spans="3:10">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E21" s="20">
         <v>3003</v>
       </c>
@@ -1353,7 +1439,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="22" spans="3:10">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E22" s="20">
         <v>3004</v>
       </c>
@@ -1369,7 +1455,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="3:10">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E23" s="20">
         <v>3005</v>
       </c>
@@ -1385,7 +1471,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="24" spans="3:10">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E24" s="20">
         <v>3006</v>
       </c>
@@ -1401,42 +1487,42 @@
         <v>370</v>
       </c>
     </row>
-    <row r="27" spans="3:10">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C27" s="21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="3:10">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C28" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="3:10">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C29" s="21" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="3:10">
+    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C30" s="21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="3:10">
+    <row r="31" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C31" s="21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="3:10">
+    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C32" s="21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="3:3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C33" s="21" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="3:3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C34" s="21" t="s">
         <v>90</v>
       </c>
@@ -1449,7 +1535,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:L4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:L4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1459,37 +1545,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="9" style="3"/>
-    <col min="3" max="3" width="49.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.25" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.453125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="26.81640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.7265625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="17.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.1796875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.54296875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="11.453125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="17.7265625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="16.7265625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="82.1796875" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="8.7265625" style="3"/>
+    <col min="6" max="6" width="7.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="26.875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.75" style="3" customWidth="1"/>
+    <col min="11" max="11" width="17.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.5" style="3" customWidth="1"/>
+    <col min="15" max="15" width="11.5" style="3" customWidth="1"/>
+    <col min="16" max="16" width="17.75" style="3" customWidth="1"/>
+    <col min="17" max="17" width="16.75" style="3" customWidth="1"/>
+    <col min="18" max="18" width="82.125" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="8.75" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1545,7 +1631,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
@@ -1599,7 +1685,7 @@
       </c>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="28">
+    <row r="4" spans="1:18" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1643,7 +1729,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1685,7 +1771,7 @@
       </c>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1727,7 +1813,7 @@
       </c>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1769,7 +1855,7 @@
       </c>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1789,7 +1875,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1809,7 +1895,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
         <v>27</v>
@@ -1861,7 +1947,7 @@
       </c>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1903,7 +1989,7 @@
       </c>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1945,7 +2031,7 @@
       </c>
       <c r="R12" s="7"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1965,7 +2051,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="7"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="6" t="s">
         <v>70</v>
@@ -2017,7 +2103,7 @@
       </c>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18" ht="28">
+    <row r="15" spans="1:18" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -2061,7 +2147,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -2081,7 +2167,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="7"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -2101,7 +2187,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="7"/>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
@@ -2149,7 +2235,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -2185,7 +2271,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -2205,7 +2291,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="7"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="6" t="s">
         <v>38</v>
@@ -2251,7 +2337,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -2287,7 +2373,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -2315,94 +2401,107 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D7:H10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B4:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:H10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="7" spans="4:8">
-      <c r="D7">
-        <v>243</v>
-      </c>
-      <c r="E7">
-        <v>333</v>
-      </c>
-      <c r="F7">
-        <v>288</v>
-      </c>
-      <c r="G7">
-        <v>63</v>
-      </c>
-      <c r="H7">
-        <v>40.5</v>
-      </c>
-    </row>
-    <row r="8" spans="4:8">
-      <c r="D8">
-        <v>323</v>
-      </c>
-      <c r="E8">
-        <v>233</v>
-      </c>
-      <c r="F8">
-        <v>53</v>
-      </c>
-      <c r="G8">
-        <v>233</v>
-      </c>
-      <c r="H8">
-        <v>30.5</v>
-      </c>
-    </row>
-    <row r="9" spans="4:8">
-      <c r="D9">
-        <f>D7+4</f>
-        <v>247</v>
-      </c>
-      <c r="E9">
-        <f t="shared" ref="E9:H10" si="0">E7+4</f>
-        <v>337</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>292</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>67</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>44.5</v>
-      </c>
-    </row>
-    <row r="10" spans="4:8">
-      <c r="D10">
-        <f>D8+4</f>
-        <v>327</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>237</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>237</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>34.5</v>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J4" t="s">
+        <v>103</v>
+      </c>
+      <c r="K4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="I6" s="22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="57" x14ac:dyDescent="0.2">
+      <c r="I8" s="22" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>